<commit_message>
Fix PCB for footprint and DRC
</commit_message>
<xml_diff>
--- a/bom/ADE7763_Bom.xlsx
+++ b/bom/ADE7763_Bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t xml:space="preserve">References</t>
   </si>
@@ -119,27 +119,6 @@
   </si>
   <si>
     <t xml:space="preserve">HC49UP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@HOLE0, @HOLE1, @HOLE2, @HOLE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOGO1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSHW-LOGOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSHW-LOGO-M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CF, INT, SAG, ZX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIREPADSMD1,27-254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD1,27-2,54</t>
   </si>
 </sst>
 </file>
@@ -154,6 +133,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -235,10 +215,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,48 +404,9 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="F10" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>4</v>
+        <f aca="false">SUM(F2:F9)</f>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>